<commit_message>
Enviamos la segunda parte de la clase del 25/05/2015
</commit_message>
<xml_diff>
--- a/IIT-25-05/PARTE I/VALIDACION DE DATOS/Alumnos-CIBERTEC.xlsx
+++ b/IIT-25-05/PARTE I/VALIDACION DE DATOS/Alumnos-CIBERTEC.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14128"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RVCBVH\Desktop\2013\2013-UCH\MATERIALES\Materiales de Excel II\EXCEL-ANALISIS Y CONTROL DE DATOS\Archivos-Primera Sesión\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235"/>
   </bookViews>
@@ -11,9 +16,8 @@
   </sheets>
   <definedNames>
     <definedName name="CURSOS">Alumnos!$N$3:$N$8</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>CÓDIGO</t>
   </si>
@@ -195,12 +199,6 @@
   </si>
   <si>
     <t>TELÉFONO</t>
-  </si>
-  <si>
-    <t>MASCULINO</t>
-  </si>
-  <si>
-    <t>FEMENINO</t>
   </si>
 </sst>
 </file>
@@ -366,36 +364,8 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7D7D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
-    </tableStyle>
-  </tableStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -450,7 +420,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
@@ -485,7 +455,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
@@ -662,7 +632,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -672,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,7 +652,7 @@
     <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
     <col min="8" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7" customWidth="1"/>
@@ -736,31 +706,17 @@
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="3">
-        <v>123456789</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="12">
-        <v>2</v>
-      </c>
-      <c r="I3" s="13">
-        <v>3</v>
-      </c>
-      <c r="J3" s="13">
-        <v>19</v>
-      </c>
-      <c r="K3" s="12">
-        <v>20</v>
-      </c>
-      <c r="L3" s="9">
+      <c r="H3" s="12"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="9" t="str">
         <f>IFERROR(ROUND(AVERAGE(H3:K3),0),"")</f>
-        <v>11</v>
+        <v/>
       </c>
       <c r="N3" s="5" t="s">
         <v>48</v>
@@ -773,12 +729,8 @@
       <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="7">
-        <v>123456789</v>
-      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="8"/>
       <c r="H4" s="14"/>
@@ -808,7 +760,10 @@
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
       <c r="K5" s="14"/>
-      <c r="L5" s="10"/>
+      <c r="L5" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="N5" s="5" t="s">
         <v>50</v>
       </c>
@@ -823,9 +778,7 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="8">
-        <v>42149</v>
-      </c>
+      <c r="G6" s="8"/>
       <c r="H6" s="14"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
@@ -923,9 +876,6 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="N10" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
@@ -946,9 +896,6 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="N11" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
@@ -959,9 +906,7 @@
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="7" t="s">
-        <v>52</v>
-      </c>
+      <c r="F12" s="7"/>
       <c r="G12" s="8"/>
       <c r="H12" s="14"/>
       <c r="I12" s="15"/>
@@ -1061,9 +1006,7 @@
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
-      <c r="F17" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="F17" s="7"/>
       <c r="G17" s="8"/>
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
@@ -1103,9 +1046,7 @@
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
-      <c r="F19" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="F19" s="7"/>
       <c r="G19" s="8"/>
       <c r="H19" s="14"/>
       <c r="I19" s="15"/>
@@ -1177,25 +1118,6 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Hey!" error="Solo debes elegir: Masculino y Femenino" sqref="D3:D22">
-      <formula1>$N$10:$N$11</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="El teléfono solo puede tener 9 caracteres" sqref="E3:E22">
-      <formula1>0</formula1>
-      <formula2>9</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:L22">
-      <formula1>0</formula1>
-      <formula2>20</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Solo los cursos listados por favor" sqref="F3:F22">
-      <formula1>CURSOS</formula1>
-    </dataValidation>
-    <dataValidation type="date" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G22">
-      <formula1>TODAY()</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>